<commit_message>
Updated Component selection spreadsheet and PCB schematics
</commit_message>
<xml_diff>
--- a/Catena di Misura/Documentation/Components Selection.xlsx
+++ b/Catena di Misura/Documentation/Components Selection.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacoi\Documents\GitHub\Electronics\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jacoi\Documents\GitHub\electronics\Catena di Misura\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D48D4C9F-8770-4BEF-B653-FDD8C348B601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A524AD-FCCA-442B-9529-B5C40D886DDA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8FD2BC0E-1192-479B-A82E-14357A549AC7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="281">
   <si>
     <t>Components Selection</t>
   </si>
@@ -924,15 +924,9 @@
     <t>Total Price</t>
   </si>
   <si>
-    <t>Omega Thermocouple Probes</t>
-  </si>
-  <si>
     <t>3mm x 200 mm</t>
   </si>
   <si>
-    <t>With Mounting Threads and M12 Connector</t>
-  </si>
-  <si>
     <t>https://www.omega.com/en-us/sensors-and-sensing-equipment/temperature/sensors/temperature-probes/probes-with-integral-connector/p/M12probes</t>
   </si>
   <si>
@@ -960,16 +954,34 @@
     <t>https://it.omega.com/pptst/M12CM.html</t>
   </si>
   <si>
-    <t>IFM Valve Plug Type A</t>
-  </si>
-  <si>
-    <t>Valve Plug Type A</t>
-  </si>
-  <si>
-    <t>A DIM</t>
-  </si>
-  <si>
-    <t>https://www.ifm.com/it/it/product/E10058</t>
+    <t>PT5423</t>
+  </si>
+  <si>
+    <t>https://www.ifm.com/it/it/product/PT5423</t>
+  </si>
+  <si>
+    <t>M12JSS-M3-U-200-E</t>
+  </si>
+  <si>
+    <t>With M8x1 Mounting Threads and M12 Connector</t>
+  </si>
+  <si>
+    <t>EVS024</t>
+  </si>
+  <si>
+    <t>Type of Cable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Right Angle M12 Cable </t>
+  </si>
+  <si>
+    <t>5m</t>
+  </si>
+  <si>
+    <t>Lenght</t>
+  </si>
+  <si>
+    <t>https://www.ifm.com/it/it/product/EVS024</t>
   </si>
 </sst>
 </file>
@@ -1056,7 +1068,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1206,13 +1218,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1276,6 +1297,7 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Collegamento ipertestuale" xfId="2" builtinId="8"/>
@@ -1592,10 +1614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15D9D64F-BE99-49AF-AE63-6321C8B28915}">
-  <dimension ref="A1:J97"/>
+  <dimension ref="A1:J98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="J77" sqref="J77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2671,11 +2693,11 @@
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+      <c r="A52" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B52" s="7">
-        <v>2</v>
+      <c r="B52" s="6">
+        <v>0</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>164</v>
@@ -2701,88 +2723,94 @@
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A53" s="25" t="s">
+      <c r="A53" s="45" t="s">
+        <v>271</v>
+      </c>
+      <c r="B53" s="7">
+        <v>2</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="H53" s="31">
+        <v>101.3</v>
+      </c>
+      <c r="I53" s="3"/>
+      <c r="J53" s="1" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A54" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="B53" s="3">
-        <f>SUM(B45:B52)</f>
+      <c r="B54" s="8">
+        <f>SUM(B45:B53)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B54" s="26">
+      <c r="B55" s="26">
         <f>(B45*H45)+(B46*H46)+(B47*H47)+(B48*H48)+(B49*H49)+(B50*H50)+(B51*H51)+(B52*H52)</f>
-        <v>202.6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A57" s="15" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A58" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="B57" s="15" t="s">
+      <c r="B58" s="15" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A58" s="22" t="s">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="B58" s="23"/>
-      <c r="C58" s="10" t="s">
+      <c r="B59" s="23"/>
+      <c r="C59" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D58" s="10" t="s">
+      <c r="D59" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E58" s="10"/>
-      <c r="F58" s="10" t="s">
+      <c r="E59" s="10"/>
+      <c r="F59" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="G58" s="10" t="s">
+      <c r="G59" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="H58" s="10" t="s">
+      <c r="H59" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="I58" s="10"/>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B59" s="5">
-        <v>0</v>
-      </c>
-      <c r="C59" s="17"/>
-      <c r="D59" s="20" t="s">
+      <c r="B60" s="5">
+        <v>0</v>
+      </c>
+      <c r="C60" s="17"/>
+      <c r="D60" s="20" t="s">
         <v>178</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="28">
-        <v>22</v>
-      </c>
-      <c r="I59" s="3"/>
-      <c r="J59" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A60" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="B60" s="6">
-        <v>0</v>
-      </c>
-      <c r="C60" s="17"/>
-      <c r="D60" s="19">
-        <v>400</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>183</v>
@@ -2790,23 +2818,23 @@
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="28">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="I60" s="3"/>
       <c r="J60" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" s="6" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B61" s="6">
         <v>0</v>
       </c>
       <c r="C61" s="17"/>
-      <c r="D61" s="20" t="s">
-        <v>186</v>
+      <c r="D61" s="19">
+        <v>400</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>183</v>
@@ -2814,13 +2842,11 @@
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="28">
-        <v>80</v>
-      </c>
-      <c r="I61" s="3" t="s">
-        <v>187</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="I61" s="3"/>
       <c r="J61" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
@@ -2832,7 +2858,7 @@
       </c>
       <c r="C62" s="17"/>
       <c r="D62" s="20" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>183</v>
@@ -2840,23 +2866,25 @@
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="28">
-        <v>37</v>
-      </c>
-      <c r="I62" s="3"/>
+        <v>80</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="J62" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" s="6" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B63" s="6">
         <v>0</v>
       </c>
       <c r="C63" s="17"/>
       <c r="D63" s="20" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>183</v>
@@ -2864,23 +2892,23 @@
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="28">
-        <v>8</v>
+        <v>37</v>
       </c>
       <c r="I63" s="3"/>
       <c r="J63" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A64" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="B64" s="7">
+      <c r="A64" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="B64" s="6">
         <v>0</v>
       </c>
       <c r="C64" s="17"/>
       <c r="D64" s="20" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>183</v>
@@ -2888,503 +2916,533 @@
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="28">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="B65" s="6">
-        <v>0</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="D65" s="24" t="s">
-        <v>209</v>
+      <c r="A65" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B65" s="7">
+        <v>0</v>
+      </c>
+      <c r="C65" s="17"/>
+      <c r="D65" s="20" t="s">
+        <v>195</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G65" s="3" t="s">
-        <v>211</v>
-      </c>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
       <c r="H65" s="28">
-        <v>8.5</v>
+        <v>40</v>
       </c>
       <c r="I65" s="3"/>
       <c r="J65" t="s">
-        <v>212</v>
+        <v>193</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A66" s="7" t="s">
-        <v>223</v>
-      </c>
-      <c r="B66" s="7">
+      <c r="A66" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B66" s="6">
         <v>0</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="D66" s="24" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>183</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="G66" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="H66" s="32">
+      <c r="H66" s="28">
+        <v>8.5</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A67" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B67" s="7">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D67" s="24" t="s">
+        <v>221</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="H67" s="32">
         <v>30</v>
       </c>
-      <c r="I66" s="3"/>
-      <c r="J66" s="1" t="s">
+      <c r="I67" s="3"/>
+      <c r="J67" s="1" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A67" s="44" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A68" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="B68" s="5">
+        <v>5</v>
+      </c>
+      <c r="C68" s="43" t="s">
         <v>261</v>
       </c>
-      <c r="B67" s="5">
-        <v>5</v>
-      </c>
-      <c r="C67" s="43" t="s">
+      <c r="D68" s="24" t="s">
+        <v>264</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="G68" s="3"/>
+      <c r="H68" s="32">
+        <v>50</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="D67" s="24" t="s">
-        <v>266</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F67" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="G67" s="3"/>
-      <c r="H67" s="32">
-        <v>50</v>
-      </c>
-      <c r="I67" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="J67" s="1" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A68" s="22" t="s">
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A69" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="22"/>
-      <c r="D68" s="18"/>
-      <c r="E68" s="18"/>
-      <c r="F68" s="18"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="18"/>
-    </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+      <c r="B69" s="22"/>
+      <c r="C69" s="22"/>
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
+      <c r="F69" s="18"/>
+      <c r="G69" s="18"/>
+      <c r="H69" s="18"/>
+      <c r="I69" s="18"/>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A70" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="B69" s="5">
-        <v>0</v>
-      </c>
-      <c r="C69" s="3" t="s">
+      <c r="B70" s="5">
+        <v>0</v>
+      </c>
+      <c r="C70" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="D69" s="24" t="s">
+      <c r="D70" s="24" t="s">
         <v>207</v>
-      </c>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3" t="s">
-        <v>199</v>
-      </c>
-      <c r="G69" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="H69" s="28">
-        <v>10</v>
-      </c>
-      <c r="I69" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="J69" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A70" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="B70" s="7">
-        <v>0</v>
-      </c>
-      <c r="C70" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D70" s="24" t="s">
-        <v>215</v>
       </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="H70" s="28">
+        <v>10</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="J70" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A71" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B71" s="7">
+        <v>0</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="E71" s="3"/>
+      <c r="F71" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G70" s="3"/>
-      <c r="H70" s="28">
+      <c r="G71" s="3"/>
+      <c r="H71" s="28">
         <v>90</v>
       </c>
-      <c r="I70" s="3" t="s">
+      <c r="I71" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="J70" t="s">
+      <c r="J71" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A71" s="25" t="s">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A72" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="B71" s="3">
-        <f>SUM(B59:B70)</f>
+      <c r="B72" s="3">
+        <f>SUM(B60:B71)</f>
         <v>5</v>
       </c>
-      <c r="D71" s="16"/>
-    </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A72" s="3" t="s">
+      <c r="D72" s="16"/>
+    </row>
+    <row r="73" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B72" s="26">
-        <f>(B62*H62)+(B63*H63)+(B64*H64)+(B65*H65)+(B66*H66)+(B67*H67)+(B69*H69)+(B70*H70)</f>
+      <c r="B73" s="26">
+        <f>(B63*H63)+(B64*H64)+(B65*H65)+(B66*H66)+(B67*H67)+(B68*H68)+(B70*H70)+(B71*H71)</f>
         <v>250</v>
       </c>
-      <c r="J72" t="s">
+      <c r="J73" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A75" s="15" t="s">
-        <v>267</v>
-      </c>
-      <c r="B75" s="15" t="s">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A76" s="15" t="s">
+        <v>265</v>
+      </c>
+      <c r="B76" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C75" s="10" t="s">
-        <v>252</v>
-      </c>
-      <c r="D75" s="10" t="s">
+      <c r="C76" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="D76" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E75" s="10" t="s">
-        <v>270</v>
-      </c>
-      <c r="F75" s="10"/>
-      <c r="G75" s="10"/>
-      <c r="H75" s="10" t="s">
+      <c r="E76" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F76" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="I75" s="10"/>
-    </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A76" s="34" t="s">
-        <v>268</v>
-      </c>
-      <c r="B76" s="34">
-        <v>1</v>
-      </c>
-      <c r="C76" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="D76" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="E76" s="3">
-        <v>2</v>
-      </c>
-      <c r="F76" s="3"/>
-      <c r="G76" s="3"/>
-      <c r="H76" s="28">
-        <v>40</v>
-      </c>
-      <c r="I76" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="J76" t="s">
-        <v>272</v>
-      </c>
+      <c r="I76" s="10"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" s="34" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B77" s="34">
         <v>1</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="E77" s="3"/>
-      <c r="F77" s="11"/>
+        <v>155</v>
+      </c>
+      <c r="E77" s="3">
+        <v>2</v>
+      </c>
+      <c r="F77" s="3"/>
       <c r="G77" s="3"/>
       <c r="H77" s="28">
-        <v>5</v>
-      </c>
-      <c r="I77" s="3"/>
-      <c r="J77" t="s">
-        <v>276</v>
+        <v>40</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A78" s="25" t="s">
+      <c r="A78" s="34" t="s">
+        <v>275</v>
+      </c>
+      <c r="B78" s="34">
+        <v>1</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E78" s="3">
+        <v>4</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>278</v>
+      </c>
+      <c r="G78" s="3"/>
+      <c r="H78" s="28">
+        <v>14.5</v>
+      </c>
+      <c r="I78" s="3"/>
+      <c r="J78" s="1" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A79" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="B78" s="3">
-        <f>SUM(B76:B77)</f>
+      <c r="B79" s="3">
+        <f>SUM(B77:B78)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A79" s="3" t="s">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B79" s="26">
-        <f>(B76*H76)+(B77*H77)</f>
-        <v>45</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A82" s="15" t="s">
+      <c r="B80" s="26">
+        <f>(B77*H77)+(B78*H78)</f>
+        <v>54.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A83" s="15" t="s">
         <v>226</v>
       </c>
-      <c r="B82" s="15" t="s">
+      <c r="B83" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C82" s="33" t="s">
+      <c r="C83" s="33" t="s">
         <v>234</v>
       </c>
-      <c r="D82" s="33" t="s">
+      <c r="D83" s="33" t="s">
         <v>235</v>
       </c>
-      <c r="E82" s="33"/>
-      <c r="F82" s="33" t="s">
+      <c r="E83" s="33"/>
+      <c r="F83" s="33" t="s">
         <v>236</v>
       </c>
-      <c r="G82" s="33" t="s">
+      <c r="G83" s="33" t="s">
         <v>243</v>
       </c>
-      <c r="H82" s="33" t="s">
+      <c r="H83" s="33" t="s">
         <v>179</v>
       </c>
-      <c r="I82" s="33" t="s">
+      <c r="I83" s="33" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A83" s="35" t="s">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A84" s="35" t="s">
         <v>230</v>
       </c>
-      <c r="B83" s="5">
-        <v>0</v>
-      </c>
-      <c r="C83" s="17" t="s">
+      <c r="B84" s="5">
+        <v>0</v>
+      </c>
+      <c r="C84" s="17" t="s">
         <v>231</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="E83" s="3"/>
-      <c r="F83" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="G83" s="3" t="s">
-        <v>242</v>
-      </c>
-      <c r="H83" s="28">
-        <v>156</v>
-      </c>
-      <c r="I83" s="3"/>
-      <c r="J83" s="1" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A84" s="36" t="s">
-        <v>238</v>
-      </c>
-      <c r="B84" s="6">
-        <v>0</v>
-      </c>
-      <c r="C84" s="17" t="s">
-        <v>239</v>
       </c>
       <c r="D84" s="3" t="s">
         <v>232</v>
       </c>
       <c r="E84" s="3"/>
       <c r="F84" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="H84" s="28">
+        <v>156</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A85" s="36" t="s">
+        <v>238</v>
+      </c>
+      <c r="B85" s="6">
+        <v>0</v>
+      </c>
+      <c r="C85" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E85" s="3"/>
+      <c r="F85" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="G84" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="H84" s="28">
+      <c r="H85" s="28">
         <v>68</v>
       </c>
-      <c r="I84" s="3" t="s">
+      <c r="I85" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="J84" t="s">
+      <c r="J85" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A85" s="37" t="s">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A86" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="B85" s="7">
+      <c r="B86" s="7">
         <v>1</v>
       </c>
-      <c r="C85" s="38" t="s">
+      <c r="C86" s="38" t="s">
         <v>247</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>248</v>
       </c>
-      <c r="E85" s="3"/>
-      <c r="F85" s="11" t="s">
+      <c r="E86" s="3"/>
+      <c r="F86" s="11" t="s">
         <v>249</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="G86" s="11" t="s">
         <v>250</v>
       </c>
-      <c r="H85" s="28">
+      <c r="H86" s="28">
         <v>114.87</v>
       </c>
-      <c r="I85" s="3"/>
-      <c r="J85" s="1" t="s">
+      <c r="I86" s="3"/>
+      <c r="J86" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A86" s="25" t="s">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A87" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="B86" s="3">
-        <f>SUM(B83:B85)</f>
+      <c r="B87" s="3">
+        <f>SUM(B84:B86)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A87" s="3" t="s">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B87" s="26">
-        <f>(B83*H83)+(B84*H84)+(B85*H85)</f>
+      <c r="B88" s="26">
+        <f>(B84*H84)+(B85*H85)+(B86*H86)</f>
         <v>114.87</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A90" s="15" t="s">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A91" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B90" s="15" t="s">
+      <c r="B91" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="C90" s="10" t="s">
+      <c r="C91" s="10" t="s">
         <v>252</v>
       </c>
-      <c r="D90" s="10" t="s">
+      <c r="D91" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="E90" s="10"/>
-      <c r="F90" s="10" t="s">
+      <c r="E91" s="10"/>
+      <c r="F91" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="G90" s="10"/>
-      <c r="H90" s="10" t="s">
+      <c r="G91" s="10"/>
+      <c r="H91" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="I90" s="10"/>
-    </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A91" s="34" t="s">
+      <c r="I91" s="10"/>
+    </row>
+    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A92" s="34" t="s">
         <v>254</v>
       </c>
-      <c r="B91" s="34">
+      <c r="B92" s="34">
         <v>1</v>
       </c>
-      <c r="C91" s="3" t="s">
+      <c r="C92" s="3" t="s">
         <v>255</v>
       </c>
-      <c r="D91" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="E91" s="3"/>
-      <c r="F91" s="3" t="s">
+      <c r="E92" s="3"/>
+      <c r="F92" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="G91" s="3"/>
-      <c r="H91" s="28">
+      <c r="G92" s="3"/>
+      <c r="H92" s="28">
         <v>10</v>
       </c>
-      <c r="I91" s="3"/>
-      <c r="J91" t="s">
+      <c r="I92" s="3"/>
+      <c r="J92" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A92" s="25" t="s">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A93" s="25" t="s">
         <v>227</v>
       </c>
-      <c r="B92" s="3">
-        <f>SUM(B91:B91)</f>
+      <c r="B93" s="3">
+        <f>SUM(B92:B92)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A93" s="3" t="s">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="B93" s="26">
-        <f>(B91*H91)</f>
+      <c r="B94" s="26">
+        <f>(B92*H92)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A96" s="39" t="s">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" s="39" t="s">
         <v>259</v>
       </c>
-      <c r="B96" s="40">
-        <f>B14+B21+B30+B40+B53+B71+B86+B78+B92</f>
+      <c r="B97" s="40">
+        <f>B14+B21+B30+B40+B54+B72+B87+B79+B93</f>
         <v>22</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A97" s="41" t="s">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" s="41" t="s">
         <v>260</v>
       </c>
-      <c r="B97" s="42">
-        <f>B15+B22+B31+B41+B54+B72+B87+B79+B93</f>
-        <v>775.97</v>
+      <c r="B98" s="42">
+        <f>B15+B22+B31+B41+B55+B73+B88+B80+B94</f>
+        <v>582.87</v>
       </c>
     </row>
   </sheetData>
@@ -3392,12 +3450,15 @@
     <hyperlink ref="J27" r:id="rId1" xr:uid="{A547992E-247C-4226-A546-82F7C2B28F04}"/>
     <hyperlink ref="J28" r:id="rId2" xr:uid="{A42014F1-C1DA-4B21-B48C-1B2F9DB27B1D}"/>
     <hyperlink ref="J52" r:id="rId3" xr:uid="{DFBA6F32-0412-4B50-811B-09BA3C1D9493}"/>
-    <hyperlink ref="J66" r:id="rId4" xr:uid="{406B602F-D266-4902-8EA9-126F2FE635A8}"/>
+    <hyperlink ref="J67" r:id="rId4" xr:uid="{406B602F-D266-4902-8EA9-126F2FE635A8}"/>
     <hyperlink ref="J29" r:id="rId5" xr:uid="{47FBED16-336B-404D-B6ED-8878D2E97D5F}"/>
-    <hyperlink ref="J83" r:id="rId6" xr:uid="{C6F3E7B8-6120-4B60-AF55-84E49BEEBBCF}"/>
-    <hyperlink ref="J85" r:id="rId7" xr:uid="{A4DC623B-F17A-4403-B85D-11475DE95F83}"/>
+    <hyperlink ref="J84" r:id="rId6" xr:uid="{C6F3E7B8-6120-4B60-AF55-84E49BEEBBCF}"/>
+    <hyperlink ref="J86" r:id="rId7" xr:uid="{A4DC623B-F17A-4403-B85D-11475DE95F83}"/>
+    <hyperlink ref="J53" r:id="rId8" xr:uid="{3AB38075-BF87-4BB3-B669-94178848CF78}"/>
+    <hyperlink ref="J78" r:id="rId9" xr:uid="{90B3AB8B-1F48-4C1F-81D7-4472F1FC1379}"/>
+    <hyperlink ref="J77" r:id="rId10" xr:uid="{A5510F36-75A4-4AA5-A785-A6ABE970DE1E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId11"/>
 </worksheet>
 </file>
</xml_diff>